<commit_message>
2017-02-13 snapshot - chunk 21
</commit_message>
<xml_diff>
--- a/www.eia.gov/petroleum/production/xls/api-history.xlsx
+++ b/www.eia.gov/petroleum/production/xls/api-history.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eianas02\OEA\MLW\Documents\EIA-914 Survey Expansion\Webpage Docs\December 2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eianas01\OES\mcr\Documents\914\2017.01_Final Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
     <sheet name="FedGOM" sheetId="17" r:id="rId18"/>
     <sheet name="OT" sheetId="18" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="152511" fullPrecision="0"/>
+  <calcPr calcId="152511" iterateDelta="9.9999999999994451E-4" fullPrecision="0"/>
 </workbook>
 </file>
 
@@ -183,10 +183,10 @@
     <t>API Category</t>
   </si>
   <si>
-    <t xml:space="preserve">Comprises states for which production data are not collected individually in the EIA-914 survey; OT includes AL, AZ, Federal Offshore Pacific, FL, IL, IN, KY, MI, MS, MO,NE, NV, NY, SD, TN, VA. </t>
+    <t>Includes: AL, AZ, Federal Offshore Pacific, FL, IL, IN, KY, MI, MS, MO, NE, NV, NY, SD, TN, VA.</t>
   </si>
   <si>
-    <t>Includes: AL, AZ, Federal Offshore Pacific, FL, IL, IN, KY, MI, MS, MO, NE, NV, NY, SD, TN, VA.</t>
+    <t xml:space="preserve">Comprises states for which production data are not collected individually in the EIA-914 report; OT includes AL, AZ, Federal Offshore Pacific, FL, IL, IN, KY, MI, MS, MO,NE, NV, NY, SD, TN, VA. </t>
   </si>
 </sst>
 </file>
@@ -308,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -342,6 +342,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -514,7 +517,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -554,7 +559,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -602,12 +607,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -618,44 +623,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -667,12 +672,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1111,7 +1116,7 @@
         <v>16</v>
       </c>
       <c r="F26" s="3">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -1122,7 +1127,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="3">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D27" s="3">
         <v>264</v>
@@ -1131,26 +1136,46 @@
         <v>13</v>
       </c>
       <c r="F27" s="3">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+        <v>409</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>122</v>
+      </c>
+      <c r="D28" s="3">
+        <v>280</v>
+      </c>
+      <c r="E28" s="3">
+        <v>15</v>
+      </c>
+      <c r="F28" s="3">
+        <v>417</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1167,11 +1192,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1182,44 +1207,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -1231,12 +1256,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1698,23 +1723,43 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>3</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
+        <v>45</v>
+      </c>
+      <c r="F28" s="3">
+        <v>48</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1731,12 +1776,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1747,44 +1792,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -1796,12 +1841,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2228,19 +2273,19 @@
         <v>42614</v>
       </c>
       <c r="B26" s="3">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="3">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D26" s="3">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E26" s="3">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F26" s="3">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2251,35 +2296,55 @@
         <v>39</v>
       </c>
       <c r="C27" s="3">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D27" s="3">
         <v>195</v>
       </c>
       <c r="E27" s="3">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F27" s="3">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+        <v>422</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>41</v>
+      </c>
+      <c r="C28" s="3">
+        <v>118</v>
+      </c>
+      <c r="D28" s="3">
+        <v>197</v>
+      </c>
+      <c r="E28" s="3">
+        <v>66</v>
+      </c>
+      <c r="F28" s="3">
+        <v>422</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2296,11 +2361,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2311,44 +2376,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -2360,12 +2425,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2827,23 +2892,43 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>15</v>
+      </c>
+      <c r="F28" s="3">
+        <v>16</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2860,12 +2945,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2876,44 +2961,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -2925,12 +3010,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -3186,10 +3271,10 @@
         <v>1632</v>
       </c>
       <c r="E17" s="3">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="F17" s="3">
-        <v>3348</v>
+        <v>3343</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="15" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -3360,16 +3445,16 @@
         <v>72</v>
       </c>
       <c r="C26" s="3">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="D26" s="3">
-        <v>1666</v>
+        <v>1662</v>
       </c>
       <c r="E26" s="3">
         <v>458</v>
       </c>
       <c r="F26" s="3">
-        <v>3159</v>
+        <v>3152</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3377,38 +3462,53 @@
         <v>42644</v>
       </c>
       <c r="B27" s="3">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C27" s="3">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="D27" s="3">
-        <v>1693</v>
+        <v>1689</v>
       </c>
       <c r="E27" s="3">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F27" s="3">
-        <v>3182</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+        <v>3175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>50</v>
+      </c>
+      <c r="C28" s="3">
+        <v>923</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1765</v>
+      </c>
+      <c r="E28" s="3">
+        <v>456</v>
+      </c>
+      <c r="F28" s="3">
+        <v>3195</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3425,12 +3525,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3441,44 +3541,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -3490,12 +3590,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -3945,7 +4045,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="3">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="3">
         <v>31</v>
@@ -3957,23 +4057,43 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>4</v>
+      </c>
+      <c r="C28" s="3">
+        <v>44</v>
+      </c>
+      <c r="D28" s="3">
+        <v>32</v>
+      </c>
+      <c r="E28" s="3">
+        <v>3</v>
+      </c>
+      <c r="F28" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3990,12 +4110,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4006,44 +4126,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -4055,12 +4175,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -4516,29 +4636,49 @@
         <v>1</v>
       </c>
       <c r="E27" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F27" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>4</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
+        <v>17</v>
+      </c>
+      <c r="F28" s="3">
+        <v>21</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4555,12 +4695,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4571,44 +4711,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -4620,12 +4760,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -5052,19 +5192,19 @@
         <v>42614</v>
       </c>
       <c r="B26" s="3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="3">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D26" s="3">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E26" s="3">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F26" s="3">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5072,38 +5212,58 @@
         <v>42644</v>
       </c>
       <c r="B27" s="3">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" s="3">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D27" s="3">
+        <v>62</v>
+      </c>
+      <c r="E27" s="3">
+        <v>37</v>
+      </c>
+      <c r="F27" s="3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>40</v>
+      </c>
+      <c r="C28" s="3">
+        <v>52</v>
+      </c>
+      <c r="D28" s="3">
         <v>64</v>
       </c>
-      <c r="E27" s="3">
-        <v>38</v>
-      </c>
-      <c r="F27" s="3">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+      <c r="E28" s="3">
+        <v>36</v>
+      </c>
+      <c r="F28" s="3">
+        <v>192</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5120,12 +5280,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5136,44 +5296,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -5185,12 +5345,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -5637,10 +5797,10 @@
         <v>42644</v>
       </c>
       <c r="B27" s="3">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="C27" s="3">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="D27" s="3">
         <v>27</v>
@@ -5649,26 +5809,46 @@
         <v>4</v>
       </c>
       <c r="F27" s="3">
-        <v>1590</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>536</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1119</v>
+      </c>
+      <c r="D28" s="3">
+        <v>22</v>
+      </c>
+      <c r="E28" s="3">
+        <v>4</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1681</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5685,12 +5865,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ30"/>
+  <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5702,44 +5882,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -5751,12 +5931,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -6189,13 +6369,13 @@
         <v>43</v>
       </c>
       <c r="D26" s="3">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E26" s="3">
         <v>14</v>
       </c>
       <c r="F26" s="3">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6203,29 +6383,49 @@
         <v>42644</v>
       </c>
       <c r="B27" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C27" s="3">
         <v>42</v>
       </c>
       <c r="D27" s="3">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E27" s="3">
         <v>14</v>
       </c>
       <c r="F27" s="3">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>46</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>33</v>
+      </c>
+      <c r="C28" s="3">
+        <v>41</v>
+      </c>
+      <c r="D28" s="3">
+        <v>71</v>
+      </c>
+      <c r="E28" s="3">
+        <v>14</v>
+      </c>
+      <c r="F28" s="3">
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -6243,12 +6443,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AP29"/>
+  <dimension ref="A1:AP30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AP1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6261,50 +6461,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="25"/>
-      <c r="AO1" s="25"/>
-      <c r="AP1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
     </row>
     <row r="2" spans="1:42" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -6316,18 +6516,18 @@
     </row>
     <row r="4" spans="1:42" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
     </row>
     <row r="5" spans="1:42" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -6811,7 +7011,7 @@
         <v>1043</v>
       </c>
       <c r="I17" s="3">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="J17" s="3">
         <v>552</v>
@@ -6820,7 +7020,7 @@
         <v>62</v>
       </c>
       <c r="L17" s="3">
-        <v>8703</v>
+        <v>8698</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="15" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7138,31 +7338,31 @@
         <v>160</v>
       </c>
       <c r="D26" s="3">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E26" s="3">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="F26" s="3">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="G26" s="3">
-        <v>2446</v>
+        <v>2463</v>
       </c>
       <c r="H26" s="3">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="I26" s="3">
-        <v>415</v>
+        <v>394</v>
       </c>
       <c r="J26" s="3">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="K26" s="3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L26" s="3">
-        <v>8123</v>
+        <v>8115</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7170,41 +7370,79 @@
         <v>42644</v>
       </c>
       <c r="B27" s="3">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="C27" s="3">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D27" s="3">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="E27" s="3">
-        <v>1188</v>
+        <v>1214</v>
       </c>
       <c r="F27" s="3">
-        <v>1595</v>
+        <v>1562</v>
       </c>
       <c r="G27" s="3">
-        <v>2515</v>
+        <v>2525</v>
       </c>
       <c r="H27" s="3">
-        <v>981</v>
+        <v>995</v>
       </c>
       <c r="I27" s="3">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="J27" s="3">
-        <v>416</v>
+        <v>397</v>
       </c>
       <c r="K27" s="3">
         <v>17</v>
       </c>
       <c r="L27" s="3">
-        <v>8312</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
+        <v>8304</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>395</v>
+      </c>
+      <c r="C28" s="3">
+        <v>163</v>
+      </c>
+      <c r="D28" s="3">
+        <v>672</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1247</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1497</v>
+      </c>
+      <c r="G28" s="3">
+        <v>2636</v>
+      </c>
+      <c r="H28" s="3">
+        <v>958</v>
+      </c>
+      <c r="I28" s="3">
+        <v>405</v>
+      </c>
+      <c r="J28" s="3">
+        <v>403</v>
+      </c>
+      <c r="K28" s="3">
+        <v>15</v>
+      </c>
+      <c r="L28" s="3">
+        <v>8391</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -7223,12 +7461,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7239,44 +7477,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -7287,12 +7525,12 @@
       <c r="A3" s="13"/>
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -7739,7 +7977,7 @@
         <v>42644</v>
       </c>
       <c r="B27" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C27" s="3">
         <v>4</v>
@@ -7754,8 +7992,28 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>4</v>
+      </c>
+      <c r="C28" s="3">
+        <v>4</v>
+      </c>
+      <c r="D28" s="3">
+        <v>6</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -7774,12 +8032,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7790,44 +8048,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -7839,12 +8097,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -8271,7 +8529,7 @@
         <v>42614</v>
       </c>
       <c r="B26" s="3">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C26" s="3">
         <v>39</v>
@@ -8306,23 +8564,43 @@
         <v>505</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>462</v>
+      </c>
+      <c r="C28" s="3">
+        <v>41</v>
+      </c>
+      <c r="D28" s="3">
+        <v>3</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>505</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8339,12 +8617,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8355,44 +8633,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -8404,12 +8682,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -8839,13 +9117,13 @@
         <v>0</v>
       </c>
       <c r="C26" s="3">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" s="3">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="E26" s="3">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="F26" s="3">
         <v>322</v>
@@ -8862,32 +9140,52 @@
         <v>50</v>
       </c>
       <c r="D27" s="3">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="E27" s="3">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="F27" s="3">
         <v>316</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3">
+        <v>49</v>
+      </c>
+      <c r="D28" s="3">
+        <v>137</v>
+      </c>
+      <c r="E28" s="3">
+        <v>120</v>
+      </c>
+      <c r="F28" s="3">
+        <v>307</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8904,12 +9202,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8920,44 +9218,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -8969,12 +9267,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -9436,23 +9734,43 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>18</v>
+      </c>
+      <c r="C28" s="3">
+        <v>63</v>
+      </c>
+      <c r="D28" s="3">
+        <v>14</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>95</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -9469,12 +9787,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9485,44 +9803,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -9534,12 +9852,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -10001,23 +10319,43 @@
         <v>153</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>28</v>
+      </c>
+      <c r="C28" s="3">
+        <v>71</v>
+      </c>
+      <c r="D28" s="3">
+        <v>34</v>
+      </c>
+      <c r="E28" s="3">
+        <v>13</v>
+      </c>
+      <c r="F28" s="3">
+        <v>145</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10034,12 +10372,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10050,44 +10388,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -10099,12 +10437,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -10566,23 +10904,43 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3">
+        <v>24</v>
+      </c>
+      <c r="D28" s="3">
+        <v>34</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>61</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10599,12 +10957,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ29"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C124" sqref="C124"/>
-      <selection pane="bottomLeft" sqref="A1:AJ1"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10615,44 +10973,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -10664,12 +11022,12 @@
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -11102,7 +11460,7 @@
         <v>91</v>
       </c>
       <c r="D26" s="3">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
@@ -11119,10 +11477,10 @@
         <v>13</v>
       </c>
       <c r="C27" s="3">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D27" s="3">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E27" s="3">
         <v>3</v>
@@ -11131,23 +11489,43 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+    <row r="28" spans="1:6" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B28" s="3">
+        <v>11</v>
+      </c>
+      <c r="C28" s="3">
+        <v>70</v>
+      </c>
+      <c r="D28" s="3">
+        <v>942</v>
+      </c>
+      <c r="E28" s="3">
+        <v>6</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1029</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>